<commit_message>
Removed overhead when clearing ranges. Refactored XLRow and XLColumn classes.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/ClearingRanges.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Ranges/ClearingRanges.xlsx
@@ -621,7 +621,6 @@
       <x:c r="G1" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="H1" s="0" t="s"/>
       <x:c r="I1" s="1" t="s">
         <x:v>4</x:v>
       </x:c>
@@ -642,7 +641,6 @@
       <x:c r="G2" s="1" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s"/>
       <x:c r="I2" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
@@ -669,7 +667,6 @@
       <x:c r="G3" s="1" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s"/>
       <x:c r="I3" s="1" t="s">
         <x:v>18</x:v>
       </x:c>
@@ -690,7 +687,6 @@
       <x:c r="G4" s="1" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="H4" s="0" t="s"/>
       <x:c r="I4" s="1" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -720,7 +716,6 @@
       <x:c r="G5" s="1" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="H5" s="0" t="s"/>
       <x:c r="I5" s="1" t="s">
         <x:v>33</x:v>
       </x:c>
@@ -750,7 +745,6 @@
       <x:c r="G6" s="1" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="H6" s="0" t="s"/>
       <x:c r="I6" s="1" t="s">
         <x:v>42</x:v>
       </x:c>
@@ -758,9 +752,7 @@
         <x:v>43</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:10">
-      <x:c r="H7" s="0" t="s"/>
-    </x:row>
+    <x:row r="7" spans="1:10"/>
     <x:row r="8" spans="1:10">
       <x:c r="A8" s="1" t="s">
         <x:v>44</x:v>

</xml_diff>